<commit_message>
Update .xlsx output files.
</commit_message>
<xml_diff>
--- a/documents/schedule_classes_zamkowa15.xlsx
+++ b/documents/schedule_classes_zamkowa15.xlsx
@@ -74,7 +74,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="25">
+  <borders count="31">
     <border>
       <left/>
       <right/>
@@ -186,6 +186,38 @@
       <right style="medium">
         <color rgb="00000000"/>
       </right>
+      <top style="medium">
+        <color rgb="00000000"/>
+      </top>
+      <bottom/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="medium">
+        <color rgb="00000000"/>
+      </right>
+      <top style="medium">
+        <color rgb="00000000"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="00000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="00000000"/>
+      </right>
+      <top style="medium">
+        <color rgb="00000000"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color rgb="00000000"/>
+      </right>
       <top/>
       <bottom style="medium">
         <color rgb="00000000"/>
@@ -212,6 +244,38 @@
       <bottom style="medium">
         <color rgb="00000000"/>
       </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="00000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="00000000"/>
+      </right>
+      <top style="medium">
+        <color rgb="00000000"/>
+      </top>
+      <bottom/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="medium">
+        <color rgb="00000000"/>
+      </right>
+      <top style="medium">
+        <color rgb="00000000"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="00000000"/>
+      </bottom>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color rgb="00000000"/>
+      </top>
+      <bottom/>
     </border>
     <border>
       <left style="thin">
@@ -311,61 +375,62 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="9" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="18" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="19" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="20" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="22" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="23" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="24" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="25" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="26" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="28" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="29" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="30" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="24" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="19" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="25" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="30" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="24" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="18" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="30" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="24" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="18" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="29" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="23" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="27" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="21" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="28" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="22" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="29" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="23" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="21" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="27" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -733,7 +798,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:W20"/>
+  <dimension ref="A1:W21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2322,6 +2387,30 @@
       <c r="V20" s="17" t="inlineStr"/>
       <c r="W20" s="18" t="inlineStr"/>
     </row>
+    <row r="21">
+      <c r="B21" s="19" t="n"/>
+      <c r="C21" s="19" t="n"/>
+      <c r="D21" s="19" t="n"/>
+      <c r="E21" s="19" t="n"/>
+      <c r="F21" s="19" t="n"/>
+      <c r="G21" s="19" t="n"/>
+      <c r="H21" s="19" t="n"/>
+      <c r="I21" s="19" t="n"/>
+      <c r="J21" s="19" t="n"/>
+      <c r="K21" s="19" t="n"/>
+      <c r="L21" s="19" t="n"/>
+      <c r="M21" s="19" t="n"/>
+      <c r="N21" s="19" t="n"/>
+      <c r="O21" s="19" t="n"/>
+      <c r="P21" s="19" t="n"/>
+      <c r="Q21" s="19" t="n"/>
+      <c r="R21" s="19" t="n"/>
+      <c r="S21" s="19" t="n"/>
+      <c r="T21" s="19" t="n"/>
+      <c r="U21" s="19" t="n"/>
+      <c r="V21" s="19" t="n"/>
+      <c r="W21" s="19" t="n"/>
+    </row>
   </sheetData>
   <mergeCells count="15">
     <mergeCell ref="B9:B10"/>
@@ -2350,7 +2439,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:W18"/>
+  <dimension ref="A1:W19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3622,48 +3711,72 @@
     </row>
     <row r="18" ht="14.3" customHeight="1">
       <c r="A18" s="2" t="n"/>
-      <c r="B18" s="19" t="n">
+      <c r="B18" s="20" t="n">
         <v>9</v>
       </c>
-      <c r="C18" s="19" t="inlineStr">
+      <c r="C18" s="20" t="inlineStr">
         <is>
           <t>15:00-15:45</t>
         </is>
       </c>
-      <c r="D18" s="20" t="inlineStr">
+      <c r="D18" s="21" t="inlineStr">
         <is>
           <t>geografia</t>
         </is>
       </c>
-      <c r="E18" s="20" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="F18" s="20" t="inlineStr">
+      <c r="E18" s="21" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F18" s="21" t="inlineStr">
         <is>
           <t>KR</t>
         </is>
       </c>
-      <c r="G18" s="21" t="n">
+      <c r="G18" s="22" t="n">
         <v>103</v>
       </c>
-      <c r="H18" s="20" t="inlineStr"/>
-      <c r="I18" s="20" t="inlineStr"/>
-      <c r="J18" s="20" t="inlineStr"/>
-      <c r="K18" s="21" t="inlineStr"/>
-      <c r="L18" s="20" t="inlineStr"/>
-      <c r="M18" s="20" t="inlineStr"/>
-      <c r="N18" s="20" t="inlineStr"/>
-      <c r="O18" s="21" t="inlineStr"/>
-      <c r="P18" s="20" t="inlineStr"/>
-      <c r="Q18" s="20" t="inlineStr"/>
-      <c r="R18" s="20" t="inlineStr"/>
-      <c r="S18" s="21" t="inlineStr"/>
-      <c r="T18" s="20" t="inlineStr"/>
-      <c r="U18" s="20" t="inlineStr"/>
-      <c r="V18" s="20" t="inlineStr"/>
-      <c r="W18" s="21" t="inlineStr"/>
+      <c r="H18" s="21" t="inlineStr"/>
+      <c r="I18" s="21" t="inlineStr"/>
+      <c r="J18" s="21" t="inlineStr"/>
+      <c r="K18" s="22" t="inlineStr"/>
+      <c r="L18" s="21" t="inlineStr"/>
+      <c r="M18" s="21" t="inlineStr"/>
+      <c r="N18" s="21" t="inlineStr"/>
+      <c r="O18" s="22" t="inlineStr"/>
+      <c r="P18" s="21" t="inlineStr"/>
+      <c r="Q18" s="21" t="inlineStr"/>
+      <c r="R18" s="21" t="inlineStr"/>
+      <c r="S18" s="22" t="inlineStr"/>
+      <c r="T18" s="21" t="inlineStr"/>
+      <c r="U18" s="21" t="inlineStr"/>
+      <c r="V18" s="21" t="inlineStr"/>
+      <c r="W18" s="22" t="inlineStr"/>
+    </row>
+    <row r="19">
+      <c r="B19" s="19" t="n"/>
+      <c r="C19" s="19" t="n"/>
+      <c r="D19" s="19" t="n"/>
+      <c r="E19" s="19" t="n"/>
+      <c r="F19" s="19" t="n"/>
+      <c r="G19" s="19" t="n"/>
+      <c r="H19" s="19" t="n"/>
+      <c r="I19" s="19" t="n"/>
+      <c r="J19" s="19" t="n"/>
+      <c r="K19" s="19" t="n"/>
+      <c r="L19" s="19" t="n"/>
+      <c r="M19" s="19" t="n"/>
+      <c r="N19" s="19" t="n"/>
+      <c r="O19" s="19" t="n"/>
+      <c r="P19" s="19" t="n"/>
+      <c r="Q19" s="19" t="n"/>
+      <c r="R19" s="19" t="n"/>
+      <c r="S19" s="19" t="n"/>
+      <c r="T19" s="19" t="n"/>
+      <c r="U19" s="19" t="n"/>
+      <c r="V19" s="19" t="n"/>
+      <c r="W19" s="19" t="n"/>
     </row>
   </sheetData>
   <mergeCells count="12">
@@ -3690,7 +3803,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:W16"/>
+  <dimension ref="A1:W17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -4557,6 +4670,30 @@
       <c r="V16" s="17" t="inlineStr"/>
       <c r="W16" s="18" t="inlineStr"/>
     </row>
+    <row r="17">
+      <c r="B17" s="19" t="n"/>
+      <c r="C17" s="19" t="n"/>
+      <c r="D17" s="19" t="n"/>
+      <c r="E17" s="19" t="n"/>
+      <c r="F17" s="19" t="n"/>
+      <c r="G17" s="19" t="n"/>
+      <c r="H17" s="19" t="n"/>
+      <c r="I17" s="19" t="n"/>
+      <c r="J17" s="19" t="n"/>
+      <c r="K17" s="19" t="n"/>
+      <c r="L17" s="19" t="n"/>
+      <c r="M17" s="19" t="n"/>
+      <c r="N17" s="19" t="n"/>
+      <c r="O17" s="19" t="n"/>
+      <c r="P17" s="19" t="n"/>
+      <c r="Q17" s="19" t="n"/>
+      <c r="R17" s="19" t="n"/>
+      <c r="S17" s="19" t="n"/>
+      <c r="T17" s="19" t="n"/>
+      <c r="U17" s="19" t="n"/>
+      <c r="V17" s="19" t="n"/>
+      <c r="W17" s="19" t="n"/>
+    </row>
   </sheetData>
   <mergeCells count="7">
     <mergeCell ref="D4:W4"/>
@@ -4577,7 +4714,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:W20"/>
+  <dimension ref="A1:W21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -6083,48 +6220,72 @@
     </row>
     <row r="20" ht="14.3" customHeight="1">
       <c r="A20" s="2" t="n"/>
-      <c r="B20" s="19" t="n">
+      <c r="B20" s="20" t="n">
         <v>9</v>
       </c>
-      <c r="C20" s="19" t="inlineStr">
+      <c r="C20" s="20" t="inlineStr">
         <is>
           <t>15:00-15:45</t>
         </is>
       </c>
-      <c r="D20" s="20" t="inlineStr"/>
-      <c r="E20" s="20" t="inlineStr"/>
-      <c r="F20" s="20" t="inlineStr"/>
-      <c r="G20" s="21" t="inlineStr"/>
-      <c r="H20" s="20" t="inlineStr"/>
-      <c r="I20" s="20" t="inlineStr"/>
-      <c r="J20" s="20" t="inlineStr"/>
-      <c r="K20" s="21" t="inlineStr"/>
-      <c r="L20" s="20" t="inlineStr">
+      <c r="D20" s="21" t="inlineStr"/>
+      <c r="E20" s="21" t="inlineStr"/>
+      <c r="F20" s="21" t="inlineStr"/>
+      <c r="G20" s="22" t="inlineStr"/>
+      <c r="H20" s="21" t="inlineStr"/>
+      <c r="I20" s="21" t="inlineStr"/>
+      <c r="J20" s="21" t="inlineStr"/>
+      <c r="K20" s="22" t="inlineStr"/>
+      <c r="L20" s="21" t="inlineStr">
         <is>
           <t>h.i.t</t>
         </is>
       </c>
-      <c r="M20" s="20" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="N20" s="20" t="inlineStr">
+      <c r="M20" s="21" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="N20" s="21" t="inlineStr">
         <is>
           <t>PA</t>
         </is>
       </c>
-      <c r="O20" s="21" t="n">
+      <c r="O20" s="22" t="n">
         <v>112</v>
       </c>
-      <c r="P20" s="20" t="inlineStr"/>
-      <c r="Q20" s="20" t="inlineStr"/>
-      <c r="R20" s="20" t="inlineStr"/>
-      <c r="S20" s="21" t="inlineStr"/>
-      <c r="T20" s="20" t="inlineStr"/>
-      <c r="U20" s="20" t="inlineStr"/>
-      <c r="V20" s="20" t="inlineStr"/>
-      <c r="W20" s="21" t="inlineStr"/>
+      <c r="P20" s="21" t="inlineStr"/>
+      <c r="Q20" s="21" t="inlineStr"/>
+      <c r="R20" s="21" t="inlineStr"/>
+      <c r="S20" s="22" t="inlineStr"/>
+      <c r="T20" s="21" t="inlineStr"/>
+      <c r="U20" s="21" t="inlineStr"/>
+      <c r="V20" s="21" t="inlineStr"/>
+      <c r="W20" s="22" t="inlineStr"/>
+    </row>
+    <row r="21">
+      <c r="B21" s="19" t="n"/>
+      <c r="C21" s="19" t="n"/>
+      <c r="D21" s="19" t="n"/>
+      <c r="E21" s="19" t="n"/>
+      <c r="F21" s="19" t="n"/>
+      <c r="G21" s="19" t="n"/>
+      <c r="H21" s="19" t="n"/>
+      <c r="I21" s="19" t="n"/>
+      <c r="J21" s="19" t="n"/>
+      <c r="K21" s="19" t="n"/>
+      <c r="L21" s="19" t="n"/>
+      <c r="M21" s="19" t="n"/>
+      <c r="N21" s="19" t="n"/>
+      <c r="O21" s="19" t="n"/>
+      <c r="P21" s="19" t="n"/>
+      <c r="Q21" s="19" t="n"/>
+      <c r="R21" s="19" t="n"/>
+      <c r="S21" s="19" t="n"/>
+      <c r="T21" s="19" t="n"/>
+      <c r="U21" s="19" t="n"/>
+      <c r="V21" s="19" t="n"/>
+      <c r="W21" s="19" t="n"/>
     </row>
   </sheetData>
   <mergeCells count="14">
@@ -6153,7 +6314,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:W13"/>
+  <dimension ref="A1:W14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -7230,90 +7391,114 @@
     </row>
     <row r="13" ht="14.3" customHeight="1">
       <c r="A13" s="2" t="n"/>
-      <c r="B13" s="19" t="n">
+      <c r="B13" s="20" t="n">
         <v>9</v>
       </c>
-      <c r="C13" s="19" t="inlineStr">
+      <c r="C13" s="20" t="inlineStr">
         <is>
           <t>15:00-15:45</t>
         </is>
       </c>
-      <c r="D13" s="20" t="inlineStr">
+      <c r="D13" s="21" t="inlineStr">
         <is>
           <t>historia</t>
         </is>
       </c>
-      <c r="E13" s="20" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="F13" s="20" t="inlineStr">
+      <c r="E13" s="21" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F13" s="21" t="inlineStr">
         <is>
           <t>PA</t>
         </is>
       </c>
-      <c r="G13" s="21" t="n">
+      <c r="G13" s="22" t="n">
         <v>112</v>
       </c>
-      <c r="H13" s="20" t="inlineStr">
+      <c r="H13" s="21" t="inlineStr">
         <is>
           <t>infor</t>
         </is>
       </c>
-      <c r="I13" s="20" t="inlineStr">
+      <c r="I13" s="21" t="inlineStr">
         <is>
           <t>1/2</t>
         </is>
       </c>
-      <c r="J13" s="20" t="inlineStr">
+      <c r="J13" s="21" t="inlineStr">
         <is>
           <t>MŚ</t>
         </is>
       </c>
-      <c r="K13" s="21" t="n">
+      <c r="K13" s="22" t="n">
         <v>109</v>
       </c>
-      <c r="L13" s="20" t="inlineStr">
+      <c r="L13" s="21" t="inlineStr">
         <is>
           <t>infor</t>
         </is>
       </c>
-      <c r="M13" s="20" t="inlineStr">
+      <c r="M13" s="21" t="inlineStr">
         <is>
           <t>2/2</t>
         </is>
       </c>
-      <c r="N13" s="20" t="inlineStr">
+      <c r="N13" s="21" t="inlineStr">
         <is>
           <t>MŚ</t>
         </is>
       </c>
-      <c r="O13" s="21" t="n">
+      <c r="O13" s="22" t="n">
         <v>109</v>
       </c>
-      <c r="P13" s="20" t="inlineStr">
+      <c r="P13" s="21" t="inlineStr">
         <is>
           <t>z.r.wło</t>
         </is>
       </c>
-      <c r="Q13" s="20" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="R13" s="20" t="inlineStr">
+      <c r="Q13" s="21" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="R13" s="21" t="inlineStr">
         <is>
           <t>PK</t>
         </is>
       </c>
-      <c r="S13" s="21" t="n">
+      <c r="S13" s="22" t="n">
         <v>202</v>
       </c>
-      <c r="T13" s="20" t="inlineStr"/>
-      <c r="U13" s="20" t="inlineStr"/>
-      <c r="V13" s="20" t="inlineStr"/>
-      <c r="W13" s="21" t="inlineStr"/>
+      <c r="T13" s="21" t="inlineStr"/>
+      <c r="U13" s="21" t="inlineStr"/>
+      <c r="V13" s="21" t="inlineStr"/>
+      <c r="W13" s="22" t="inlineStr"/>
+    </row>
+    <row r="14">
+      <c r="B14" s="19" t="n"/>
+      <c r="C14" s="19" t="n"/>
+      <c r="D14" s="19" t="n"/>
+      <c r="E14" s="19" t="n"/>
+      <c r="F14" s="19" t="n"/>
+      <c r="G14" s="19" t="n"/>
+      <c r="H14" s="19" t="n"/>
+      <c r="I14" s="19" t="n"/>
+      <c r="J14" s="19" t="n"/>
+      <c r="K14" s="19" t="n"/>
+      <c r="L14" s="19" t="n"/>
+      <c r="M14" s="19" t="n"/>
+      <c r="N14" s="19" t="n"/>
+      <c r="O14" s="19" t="n"/>
+      <c r="P14" s="19" t="n"/>
+      <c r="Q14" s="19" t="n"/>
+      <c r="R14" s="19" t="n"/>
+      <c r="S14" s="19" t="n"/>
+      <c r="T14" s="19" t="n"/>
+      <c r="U14" s="19" t="n"/>
+      <c r="V14" s="19" t="n"/>
+      <c r="W14" s="19" t="n"/>
     </row>
   </sheetData>
   <mergeCells count="7">
@@ -7335,7 +7520,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:W14"/>
+  <dimension ref="A1:W15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -8138,6 +8323,30 @@
       <c r="V14" s="17" t="inlineStr"/>
       <c r="W14" s="18" t="inlineStr"/>
     </row>
+    <row r="15">
+      <c r="B15" s="19" t="n"/>
+      <c r="C15" s="19" t="n"/>
+      <c r="D15" s="19" t="n"/>
+      <c r="E15" s="19" t="n"/>
+      <c r="F15" s="19" t="n"/>
+      <c r="G15" s="19" t="n"/>
+      <c r="H15" s="19" t="n"/>
+      <c r="I15" s="19" t="n"/>
+      <c r="J15" s="19" t="n"/>
+      <c r="K15" s="19" t="n"/>
+      <c r="L15" s="19" t="n"/>
+      <c r="M15" s="19" t="n"/>
+      <c r="N15" s="19" t="n"/>
+      <c r="O15" s="19" t="n"/>
+      <c r="P15" s="19" t="n"/>
+      <c r="Q15" s="19" t="n"/>
+      <c r="R15" s="19" t="n"/>
+      <c r="S15" s="19" t="n"/>
+      <c r="T15" s="19" t="n"/>
+      <c r="U15" s="19" t="n"/>
+      <c r="V15" s="19" t="n"/>
+      <c r="W15" s="19" t="n"/>
+    </row>
   </sheetData>
   <mergeCells count="9">
     <mergeCell ref="D4:W4"/>
@@ -8160,7 +8369,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:W14"/>
+  <dimension ref="A1:W15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -8963,6 +9172,30 @@
         </is>
       </c>
     </row>
+    <row r="15">
+      <c r="B15" s="19" t="n"/>
+      <c r="C15" s="19" t="n"/>
+      <c r="D15" s="19" t="n"/>
+      <c r="E15" s="19" t="n"/>
+      <c r="F15" s="19" t="n"/>
+      <c r="G15" s="19" t="n"/>
+      <c r="H15" s="19" t="n"/>
+      <c r="I15" s="19" t="n"/>
+      <c r="J15" s="19" t="n"/>
+      <c r="K15" s="19" t="n"/>
+      <c r="L15" s="19" t="n"/>
+      <c r="M15" s="19" t="n"/>
+      <c r="N15" s="19" t="n"/>
+      <c r="O15" s="19" t="n"/>
+      <c r="P15" s="19" t="n"/>
+      <c r="Q15" s="19" t="n"/>
+      <c r="R15" s="19" t="n"/>
+      <c r="S15" s="19" t="n"/>
+      <c r="T15" s="19" t="n"/>
+      <c r="U15" s="19" t="n"/>
+      <c r="V15" s="19" t="n"/>
+      <c r="W15" s="19" t="n"/>
+    </row>
   </sheetData>
   <mergeCells count="9">
     <mergeCell ref="D4:W4"/>
@@ -8985,7 +9218,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:W20"/>
+  <dimension ref="A1:W21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -10503,48 +10736,72 @@
     </row>
     <row r="20" ht="14.3" customHeight="1">
       <c r="A20" s="2" t="n"/>
-      <c r="B20" s="19" t="n">
+      <c r="B20" s="20" t="n">
         <v>9</v>
       </c>
-      <c r="C20" s="19" t="inlineStr">
+      <c r="C20" s="20" t="inlineStr">
         <is>
           <t>15:00-15:45</t>
         </is>
       </c>
-      <c r="D20" s="20" t="inlineStr"/>
-      <c r="E20" s="20" t="inlineStr"/>
-      <c r="F20" s="20" t="inlineStr"/>
-      <c r="G20" s="21" t="inlineStr"/>
-      <c r="H20" s="20" t="inlineStr">
+      <c r="D20" s="21" t="inlineStr"/>
+      <c r="E20" s="21" t="inlineStr"/>
+      <c r="F20" s="21" t="inlineStr"/>
+      <c r="G20" s="22" t="inlineStr"/>
+      <c r="H20" s="21" t="inlineStr">
         <is>
           <t>ang</t>
         </is>
       </c>
-      <c r="I20" s="20" t="inlineStr">
+      <c r="I20" s="21" t="inlineStr">
         <is>
           <t>ra</t>
         </is>
       </c>
-      <c r="J20" s="20" t="inlineStr">
+      <c r="J20" s="21" t="inlineStr">
         <is>
           <t>PS</t>
         </is>
       </c>
-      <c r="K20" s="21" t="n">
+      <c r="K20" s="22" t="n">
         <v>210</v>
       </c>
-      <c r="L20" s="20" t="inlineStr"/>
-      <c r="M20" s="20" t="inlineStr"/>
-      <c r="N20" s="20" t="inlineStr"/>
-      <c r="O20" s="21" t="inlineStr"/>
-      <c r="P20" s="20" t="inlineStr"/>
-      <c r="Q20" s="20" t="inlineStr"/>
-      <c r="R20" s="20" t="inlineStr"/>
-      <c r="S20" s="21" t="inlineStr"/>
-      <c r="T20" s="20" t="inlineStr"/>
-      <c r="U20" s="20" t="inlineStr"/>
-      <c r="V20" s="20" t="inlineStr"/>
-      <c r="W20" s="21" t="inlineStr"/>
+      <c r="L20" s="21" t="inlineStr"/>
+      <c r="M20" s="21" t="inlineStr"/>
+      <c r="N20" s="21" t="inlineStr"/>
+      <c r="O20" s="22" t="inlineStr"/>
+      <c r="P20" s="21" t="inlineStr"/>
+      <c r="Q20" s="21" t="inlineStr"/>
+      <c r="R20" s="21" t="inlineStr"/>
+      <c r="S20" s="22" t="inlineStr"/>
+      <c r="T20" s="21" t="inlineStr"/>
+      <c r="U20" s="21" t="inlineStr"/>
+      <c r="V20" s="21" t="inlineStr"/>
+      <c r="W20" s="22" t="inlineStr"/>
+    </row>
+    <row r="21">
+      <c r="B21" s="19" t="n"/>
+      <c r="C21" s="19" t="n"/>
+      <c r="D21" s="19" t="n"/>
+      <c r="E21" s="19" t="n"/>
+      <c r="F21" s="19" t="n"/>
+      <c r="G21" s="19" t="n"/>
+      <c r="H21" s="19" t="n"/>
+      <c r="I21" s="19" t="n"/>
+      <c r="J21" s="19" t="n"/>
+      <c r="K21" s="19" t="n"/>
+      <c r="L21" s="19" t="n"/>
+      <c r="M21" s="19" t="n"/>
+      <c r="N21" s="19" t="n"/>
+      <c r="O21" s="19" t="n"/>
+      <c r="P21" s="19" t="n"/>
+      <c r="Q21" s="19" t="n"/>
+      <c r="R21" s="19" t="n"/>
+      <c r="S21" s="19" t="n"/>
+      <c r="T21" s="19" t="n"/>
+      <c r="U21" s="19" t="n"/>
+      <c r="V21" s="19" t="n"/>
+      <c r="W21" s="19" t="n"/>
     </row>
   </sheetData>
   <mergeCells count="14">
@@ -10573,7 +10830,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:W25"/>
+  <dimension ref="A1:W26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -12456,50 +12713,74 @@
     </row>
     <row r="25" ht="14.3" customHeight="1">
       <c r="A25" s="2" t="n"/>
-      <c r="B25" s="19" t="n">
+      <c r="B25" s="20" t="n">
         <v>11</v>
       </c>
-      <c r="C25" s="19" t="inlineStr">
+      <c r="C25" s="20" t="inlineStr">
         <is>
           <t>16:40-17:25</t>
         </is>
       </c>
-      <c r="D25" s="20" t="inlineStr"/>
-      <c r="E25" s="20" t="inlineStr"/>
-      <c r="F25" s="20" t="inlineStr"/>
-      <c r="G25" s="21" t="inlineStr"/>
-      <c r="H25" s="20" t="inlineStr"/>
-      <c r="I25" s="20" t="inlineStr"/>
-      <c r="J25" s="20" t="inlineStr"/>
-      <c r="K25" s="21" t="inlineStr"/>
-      <c r="L25" s="20" t="inlineStr">
+      <c r="D25" s="21" t="inlineStr"/>
+      <c r="E25" s="21" t="inlineStr"/>
+      <c r="F25" s="21" t="inlineStr"/>
+      <c r="G25" s="22" t="inlineStr"/>
+      <c r="H25" s="21" t="inlineStr"/>
+      <c r="I25" s="21" t="inlineStr"/>
+      <c r="J25" s="21" t="inlineStr"/>
+      <c r="K25" s="22" t="inlineStr"/>
+      <c r="L25" s="21" t="inlineStr">
         <is>
           <t>pr.fry-M</t>
         </is>
       </c>
-      <c r="M25" s="20" t="inlineStr">
+      <c r="M25" s="21" t="inlineStr">
         <is>
           <t>fry</t>
         </is>
       </c>
-      <c r="N25" s="20" t="inlineStr">
+      <c r="N25" s="21" t="inlineStr">
         <is>
           <t>JG</t>
         </is>
       </c>
-      <c r="O25" s="21" t="inlineStr">
+      <c r="O25" s="22" t="inlineStr">
         <is>
           <t>_08</t>
         </is>
       </c>
-      <c r="P25" s="20" t="inlineStr"/>
-      <c r="Q25" s="20" t="inlineStr"/>
-      <c r="R25" s="20" t="inlineStr"/>
-      <c r="S25" s="21" t="inlineStr"/>
-      <c r="T25" s="20" t="inlineStr"/>
-      <c r="U25" s="20" t="inlineStr"/>
-      <c r="V25" s="20" t="inlineStr"/>
-      <c r="W25" s="21" t="inlineStr"/>
+      <c r="P25" s="21" t="inlineStr"/>
+      <c r="Q25" s="21" t="inlineStr"/>
+      <c r="R25" s="21" t="inlineStr"/>
+      <c r="S25" s="22" t="inlineStr"/>
+      <c r="T25" s="21" t="inlineStr"/>
+      <c r="U25" s="21" t="inlineStr"/>
+      <c r="V25" s="21" t="inlineStr"/>
+      <c r="W25" s="22" t="inlineStr"/>
+    </row>
+    <row r="26">
+      <c r="B26" s="19" t="n"/>
+      <c r="C26" s="19" t="n"/>
+      <c r="D26" s="19" t="n"/>
+      <c r="E26" s="19" t="n"/>
+      <c r="F26" s="19" t="n"/>
+      <c r="G26" s="19" t="n"/>
+      <c r="H26" s="19" t="n"/>
+      <c r="I26" s="19" t="n"/>
+      <c r="J26" s="19" t="n"/>
+      <c r="K26" s="19" t="n"/>
+      <c r="L26" s="19" t="n"/>
+      <c r="M26" s="19" t="n"/>
+      <c r="N26" s="19" t="n"/>
+      <c r="O26" s="19" t="n"/>
+      <c r="P26" s="19" t="n"/>
+      <c r="Q26" s="19" t="n"/>
+      <c r="R26" s="19" t="n"/>
+      <c r="S26" s="19" t="n"/>
+      <c r="T26" s="19" t="n"/>
+      <c r="U26" s="19" t="n"/>
+      <c r="V26" s="19" t="n"/>
+      <c r="W26" s="19" t="n"/>
     </row>
   </sheetData>
   <mergeCells count="15">
@@ -12529,7 +12810,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:W15"/>
+  <dimension ref="A1:W16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -13528,78 +13809,102 @@
     </row>
     <row r="15" ht="14.3" customHeight="1">
       <c r="A15" s="2" t="n"/>
-      <c r="B15" s="19" t="n">
+      <c r="B15" s="20" t="n">
         <v>7</v>
       </c>
-      <c r="C15" s="19" t="inlineStr">
+      <c r="C15" s="20" t="inlineStr">
         <is>
           <t>13:10-13:55</t>
         </is>
       </c>
-      <c r="D15" s="20" t="inlineStr">
+      <c r="D15" s="21" t="inlineStr">
         <is>
           <t>ang</t>
         </is>
       </c>
-      <c r="E15" s="20" t="inlineStr">
+      <c r="E15" s="21" t="inlineStr">
         <is>
           <t>ek</t>
         </is>
       </c>
-      <c r="F15" s="20" t="inlineStr">
+      <c r="F15" s="21" t="inlineStr">
         <is>
           <t>PS</t>
         </is>
       </c>
-      <c r="G15" s="21" t="n">
+      <c r="G15" s="22" t="n">
         <v>210</v>
       </c>
-      <c r="H15" s="20" t="inlineStr"/>
-      <c r="I15" s="20" t="inlineStr"/>
-      <c r="J15" s="20" t="inlineStr"/>
-      <c r="K15" s="21" t="inlineStr"/>
-      <c r="L15" s="20" t="inlineStr">
+      <c r="H15" s="21" t="inlineStr"/>
+      <c r="I15" s="21" t="inlineStr"/>
+      <c r="J15" s="21" t="inlineStr"/>
+      <c r="K15" s="22" t="inlineStr"/>
+      <c r="L15" s="21" t="inlineStr">
         <is>
           <t>z.z.w</t>
         </is>
       </c>
-      <c r="M15" s="20" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="N15" s="20" t="inlineStr">
+      <c r="M15" s="21" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="N15" s="21" t="inlineStr">
         <is>
           <t>PA</t>
         </is>
       </c>
-      <c r="O15" s="21" t="n">
+      <c r="O15" s="22" t="n">
         <v>112</v>
       </c>
-      <c r="P15" s="20" t="inlineStr">
+      <c r="P15" s="21" t="inlineStr">
         <is>
           <t>w.f</t>
         </is>
       </c>
-      <c r="Q15" s="20" t="inlineStr">
+      <c r="Q15" s="21" t="inlineStr">
         <is>
           <t>ek</t>
         </is>
       </c>
-      <c r="R15" s="20" t="inlineStr">
+      <c r="R15" s="21" t="inlineStr">
         <is>
           <t>MG</t>
         </is>
       </c>
-      <c r="S15" s="21" t="inlineStr">
+      <c r="S15" s="22" t="inlineStr">
         <is>
           <t>s3</t>
         </is>
       </c>
-      <c r="T15" s="20" t="inlineStr"/>
-      <c r="U15" s="20" t="inlineStr"/>
-      <c r="V15" s="20" t="inlineStr"/>
-      <c r="W15" s="21" t="inlineStr"/>
+      <c r="T15" s="21" t="inlineStr"/>
+      <c r="U15" s="21" t="inlineStr"/>
+      <c r="V15" s="21" t="inlineStr"/>
+      <c r="W15" s="22" t="inlineStr"/>
+    </row>
+    <row r="16">
+      <c r="B16" s="19" t="n"/>
+      <c r="C16" s="19" t="n"/>
+      <c r="D16" s="19" t="n"/>
+      <c r="E16" s="19" t="n"/>
+      <c r="F16" s="19" t="n"/>
+      <c r="G16" s="19" t="n"/>
+      <c r="H16" s="19" t="n"/>
+      <c r="I16" s="19" t="n"/>
+      <c r="J16" s="19" t="n"/>
+      <c r="K16" s="19" t="n"/>
+      <c r="L16" s="19" t="n"/>
+      <c r="M16" s="19" t="n"/>
+      <c r="N16" s="19" t="n"/>
+      <c r="O16" s="19" t="n"/>
+      <c r="P16" s="19" t="n"/>
+      <c r="Q16" s="19" t="n"/>
+      <c r="R16" s="19" t="n"/>
+      <c r="S16" s="19" t="n"/>
+      <c r="T16" s="19" t="n"/>
+      <c r="U16" s="19" t="n"/>
+      <c r="V16" s="19" t="n"/>
+      <c r="W16" s="19" t="n"/>
     </row>
   </sheetData>
   <mergeCells count="11">
@@ -13625,7 +13930,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:W17"/>
+  <dimension ref="A1:W18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -14716,48 +15021,72 @@
     </row>
     <row r="17" ht="14.3" customHeight="1">
       <c r="A17" s="2" t="n"/>
-      <c r="B17" s="19" t="n"/>
-      <c r="C17" s="19" t="inlineStr">
+      <c r="B17" s="20" t="n"/>
+      <c r="C17" s="20" t="inlineStr">
         <is>
           <t>15:00-15:45</t>
         </is>
       </c>
-      <c r="D17" s="20" t="inlineStr"/>
-      <c r="E17" s="20" t="inlineStr"/>
-      <c r="F17" s="20" t="inlineStr"/>
-      <c r="G17" s="21" t="inlineStr"/>
-      <c r="H17" s="20" t="inlineStr">
+      <c r="D17" s="21" t="inlineStr"/>
+      <c r="E17" s="21" t="inlineStr"/>
+      <c r="F17" s="21" t="inlineStr"/>
+      <c r="G17" s="22" t="inlineStr"/>
+      <c r="H17" s="21" t="inlineStr">
         <is>
           <t>w.f</t>
         </is>
       </c>
-      <c r="I17" s="20" t="inlineStr">
+      <c r="I17" s="21" t="inlineStr">
         <is>
           <t>fry</t>
         </is>
       </c>
-      <c r="J17" s="20" t="inlineStr">
+      <c r="J17" s="21" t="inlineStr">
         <is>
           <t>RB</t>
         </is>
       </c>
-      <c r="K17" s="21" t="inlineStr">
+      <c r="K17" s="22" t="inlineStr">
         <is>
           <t>s1</t>
         </is>
       </c>
-      <c r="L17" s="20" t="inlineStr"/>
-      <c r="M17" s="20" t="inlineStr"/>
-      <c r="N17" s="20" t="inlineStr"/>
-      <c r="O17" s="21" t="inlineStr"/>
-      <c r="P17" s="20" t="inlineStr"/>
-      <c r="Q17" s="20" t="inlineStr"/>
-      <c r="R17" s="20" t="inlineStr"/>
-      <c r="S17" s="21" t="inlineStr"/>
-      <c r="T17" s="20" t="inlineStr"/>
-      <c r="U17" s="20" t="inlineStr"/>
-      <c r="V17" s="20" t="inlineStr"/>
-      <c r="W17" s="21" t="inlineStr"/>
+      <c r="L17" s="21" t="inlineStr"/>
+      <c r="M17" s="21" t="inlineStr"/>
+      <c r="N17" s="21" t="inlineStr"/>
+      <c r="O17" s="22" t="inlineStr"/>
+      <c r="P17" s="21" t="inlineStr"/>
+      <c r="Q17" s="21" t="inlineStr"/>
+      <c r="R17" s="21" t="inlineStr"/>
+      <c r="S17" s="22" t="inlineStr"/>
+      <c r="T17" s="21" t="inlineStr"/>
+      <c r="U17" s="21" t="inlineStr"/>
+      <c r="V17" s="21" t="inlineStr"/>
+      <c r="W17" s="22" t="inlineStr"/>
+    </row>
+    <row r="18">
+      <c r="B18" s="19" t="n"/>
+      <c r="C18" s="19" t="n"/>
+      <c r="D18" s="19" t="n"/>
+      <c r="E18" s="19" t="n"/>
+      <c r="F18" s="19" t="n"/>
+      <c r="G18" s="19" t="n"/>
+      <c r="H18" s="19" t="n"/>
+      <c r="I18" s="19" t="n"/>
+      <c r="J18" s="19" t="n"/>
+      <c r="K18" s="19" t="n"/>
+      <c r="L18" s="19" t="n"/>
+      <c r="M18" s="19" t="n"/>
+      <c r="N18" s="19" t="n"/>
+      <c r="O18" s="19" t="n"/>
+      <c r="P18" s="19" t="n"/>
+      <c r="Q18" s="19" t="n"/>
+      <c r="R18" s="19" t="n"/>
+      <c r="S18" s="19" t="n"/>
+      <c r="T18" s="19" t="n"/>
+      <c r="U18" s="19" t="n"/>
+      <c r="V18" s="19" t="n"/>
+      <c r="W18" s="19" t="n"/>
     </row>
   </sheetData>
   <mergeCells count="11">
@@ -14783,7 +15112,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:W14"/>
+  <dimension ref="A1:W15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -15639,62 +15968,86 @@
     </row>
     <row r="14" ht="14.3" customHeight="1">
       <c r="A14" s="2" t="n"/>
-      <c r="B14" s="19" t="n">
+      <c r="B14" s="20" t="n">
         <v>7</v>
       </c>
-      <c r="C14" s="19" t="inlineStr">
+      <c r="C14" s="20" t="inlineStr">
         <is>
           <t>13:10-13:55</t>
         </is>
       </c>
-      <c r="D14" s="20" t="inlineStr">
+      <c r="D14" s="21" t="inlineStr">
         <is>
           <t>jęz.polski</t>
         </is>
       </c>
-      <c r="E14" s="20" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="F14" s="20" t="inlineStr">
+      <c r="E14" s="21" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F14" s="21" t="inlineStr">
         <is>
           <t>SZ</t>
         </is>
       </c>
-      <c r="G14" s="21" t="n">
+      <c r="G14" s="22" t="n">
         <v>112</v>
       </c>
-      <c r="H14" s="20" t="inlineStr"/>
-      <c r="I14" s="20" t="inlineStr"/>
-      <c r="J14" s="20" t="inlineStr"/>
-      <c r="K14" s="21" t="inlineStr"/>
-      <c r="L14" s="20" t="inlineStr">
+      <c r="H14" s="21" t="inlineStr"/>
+      <c r="I14" s="21" t="inlineStr"/>
+      <c r="J14" s="21" t="inlineStr"/>
+      <c r="K14" s="22" t="inlineStr"/>
+      <c r="L14" s="21" t="inlineStr">
         <is>
           <t>religia</t>
         </is>
       </c>
-      <c r="M14" s="20" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="N14" s="20" t="inlineStr">
+      <c r="M14" s="21" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="N14" s="21" t="inlineStr">
         <is>
           <t>DD</t>
         </is>
       </c>
-      <c r="O14" s="21" t="n">
+      <c r="O14" s="22" t="n">
         <v>116</v>
       </c>
-      <c r="P14" s="20" t="inlineStr"/>
-      <c r="Q14" s="20" t="inlineStr"/>
-      <c r="R14" s="20" t="inlineStr"/>
-      <c r="S14" s="21" t="inlineStr"/>
-      <c r="T14" s="20" t="inlineStr"/>
-      <c r="U14" s="20" t="inlineStr"/>
-      <c r="V14" s="20" t="inlineStr"/>
-      <c r="W14" s="21" t="inlineStr"/>
+      <c r="P14" s="21" t="inlineStr"/>
+      <c r="Q14" s="21" t="inlineStr"/>
+      <c r="R14" s="21" t="inlineStr"/>
+      <c r="S14" s="22" t="inlineStr"/>
+      <c r="T14" s="21" t="inlineStr"/>
+      <c r="U14" s="21" t="inlineStr"/>
+      <c r="V14" s="21" t="inlineStr"/>
+      <c r="W14" s="22" t="inlineStr"/>
+    </row>
+    <row r="15">
+      <c r="B15" s="19" t="n"/>
+      <c r="C15" s="19" t="n"/>
+      <c r="D15" s="19" t="n"/>
+      <c r="E15" s="19" t="n"/>
+      <c r="F15" s="19" t="n"/>
+      <c r="G15" s="19" t="n"/>
+      <c r="H15" s="19" t="n"/>
+      <c r="I15" s="19" t="n"/>
+      <c r="J15" s="19" t="n"/>
+      <c r="K15" s="19" t="n"/>
+      <c r="L15" s="19" t="n"/>
+      <c r="M15" s="19" t="n"/>
+      <c r="N15" s="19" t="n"/>
+      <c r="O15" s="19" t="n"/>
+      <c r="P15" s="19" t="n"/>
+      <c r="Q15" s="19" t="n"/>
+      <c r="R15" s="19" t="n"/>
+      <c r="S15" s="19" t="n"/>
+      <c r="T15" s="19" t="n"/>
+      <c r="U15" s="19" t="n"/>
+      <c r="V15" s="19" t="n"/>
+      <c r="W15" s="19" t="n"/>
     </row>
   </sheetData>
   <mergeCells count="10">
@@ -15719,7 +16072,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:W14"/>
+  <dimension ref="A1:W15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -16434,6 +16787,30 @@
       <c r="V14" s="17" t="inlineStr"/>
       <c r="W14" s="18" t="inlineStr"/>
     </row>
+    <row r="15">
+      <c r="B15" s="19" t="n"/>
+      <c r="C15" s="19" t="n"/>
+      <c r="D15" s="19" t="n"/>
+      <c r="E15" s="19" t="n"/>
+      <c r="F15" s="19" t="n"/>
+      <c r="G15" s="19" t="n"/>
+      <c r="H15" s="19" t="n"/>
+      <c r="I15" s="19" t="n"/>
+      <c r="J15" s="19" t="n"/>
+      <c r="K15" s="19" t="n"/>
+      <c r="L15" s="19" t="n"/>
+      <c r="M15" s="19" t="n"/>
+      <c r="N15" s="19" t="n"/>
+      <c r="O15" s="19" t="n"/>
+      <c r="P15" s="19" t="n"/>
+      <c r="Q15" s="19" t="n"/>
+      <c r="R15" s="19" t="n"/>
+      <c r="S15" s="19" t="n"/>
+      <c r="T15" s="19" t="n"/>
+      <c r="U15" s="19" t="n"/>
+      <c r="V15" s="19" t="n"/>
+      <c r="W15" s="19" t="n"/>
+    </row>
   </sheetData>
   <mergeCells count="7">
     <mergeCell ref="D4:W4"/>
@@ -16454,7 +16831,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:W14"/>
+  <dimension ref="A1:W15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -17179,6 +17556,30 @@
       <c r="V14" s="17" t="inlineStr"/>
       <c r="W14" s="18" t="inlineStr"/>
     </row>
+    <row r="15">
+      <c r="B15" s="19" t="n"/>
+      <c r="C15" s="19" t="n"/>
+      <c r="D15" s="19" t="n"/>
+      <c r="E15" s="19" t="n"/>
+      <c r="F15" s="19" t="n"/>
+      <c r="G15" s="19" t="n"/>
+      <c r="H15" s="19" t="n"/>
+      <c r="I15" s="19" t="n"/>
+      <c r="J15" s="19" t="n"/>
+      <c r="K15" s="19" t="n"/>
+      <c r="L15" s="19" t="n"/>
+      <c r="M15" s="19" t="n"/>
+      <c r="N15" s="19" t="n"/>
+      <c r="O15" s="19" t="n"/>
+      <c r="P15" s="19" t="n"/>
+      <c r="Q15" s="19" t="n"/>
+      <c r="R15" s="19" t="n"/>
+      <c r="S15" s="19" t="n"/>
+      <c r="T15" s="19" t="n"/>
+      <c r="U15" s="19" t="n"/>
+      <c r="V15" s="19" t="n"/>
+      <c r="W15" s="19" t="n"/>
+    </row>
   </sheetData>
   <mergeCells count="7">
     <mergeCell ref="D4:W4"/>
@@ -17199,7 +17600,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:W11"/>
+  <dimension ref="A1:W12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -17830,48 +18231,72 @@
     </row>
     <row r="11" ht="14.3" customHeight="1">
       <c r="A11" s="2" t="n"/>
-      <c r="B11" s="19" t="n">
+      <c r="B11" s="20" t="n">
         <v>7</v>
       </c>
-      <c r="C11" s="19" t="inlineStr">
+      <c r="C11" s="20" t="inlineStr">
         <is>
           <t>13:10-13:55</t>
         </is>
       </c>
-      <c r="D11" s="20" t="inlineStr">
+      <c r="D11" s="21" t="inlineStr">
         <is>
           <t>geografia</t>
         </is>
       </c>
-      <c r="E11" s="20" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="F11" s="20" t="inlineStr">
+      <c r="E11" s="21" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F11" s="21" t="inlineStr">
         <is>
           <t>KR</t>
         </is>
       </c>
-      <c r="G11" s="21" t="n">
+      <c r="G11" s="22" t="n">
         <v>6</v>
       </c>
-      <c r="H11" s="20" t="inlineStr"/>
-      <c r="I11" s="20" t="inlineStr"/>
-      <c r="J11" s="20" t="inlineStr"/>
-      <c r="K11" s="21" t="inlineStr"/>
-      <c r="L11" s="20" t="inlineStr"/>
-      <c r="M11" s="20" t="inlineStr"/>
-      <c r="N11" s="20" t="inlineStr"/>
-      <c r="O11" s="21" t="inlineStr"/>
-      <c r="P11" s="20" t="inlineStr"/>
-      <c r="Q11" s="20" t="inlineStr"/>
-      <c r="R11" s="20" t="inlineStr"/>
-      <c r="S11" s="21" t="inlineStr"/>
-      <c r="T11" s="20" t="inlineStr"/>
-      <c r="U11" s="20" t="inlineStr"/>
-      <c r="V11" s="20" t="inlineStr"/>
-      <c r="W11" s="21" t="inlineStr"/>
+      <c r="H11" s="21" t="inlineStr"/>
+      <c r="I11" s="21" t="inlineStr"/>
+      <c r="J11" s="21" t="inlineStr"/>
+      <c r="K11" s="22" t="inlineStr"/>
+      <c r="L11" s="21" t="inlineStr"/>
+      <c r="M11" s="21" t="inlineStr"/>
+      <c r="N11" s="21" t="inlineStr"/>
+      <c r="O11" s="22" t="inlineStr"/>
+      <c r="P11" s="21" t="inlineStr"/>
+      <c r="Q11" s="21" t="inlineStr"/>
+      <c r="R11" s="21" t="inlineStr"/>
+      <c r="S11" s="22" t="inlineStr"/>
+      <c r="T11" s="21" t="inlineStr"/>
+      <c r="U11" s="21" t="inlineStr"/>
+      <c r="V11" s="21" t="inlineStr"/>
+      <c r="W11" s="22" t="inlineStr"/>
+    </row>
+    <row r="12">
+      <c r="B12" s="19" t="n"/>
+      <c r="C12" s="19" t="n"/>
+      <c r="D12" s="19" t="n"/>
+      <c r="E12" s="19" t="n"/>
+      <c r="F12" s="19" t="n"/>
+      <c r="G12" s="19" t="n"/>
+      <c r="H12" s="19" t="n"/>
+      <c r="I12" s="19" t="n"/>
+      <c r="J12" s="19" t="n"/>
+      <c r="K12" s="19" t="n"/>
+      <c r="L12" s="19" t="n"/>
+      <c r="M12" s="19" t="n"/>
+      <c r="N12" s="19" t="n"/>
+      <c r="O12" s="19" t="n"/>
+      <c r="P12" s="19" t="n"/>
+      <c r="Q12" s="19" t="n"/>
+      <c r="R12" s="19" t="n"/>
+      <c r="S12" s="19" t="n"/>
+      <c r="T12" s="19" t="n"/>
+      <c r="U12" s="19" t="n"/>
+      <c r="V12" s="19" t="n"/>
+      <c r="W12" s="19" t="n"/>
     </row>
   </sheetData>
   <mergeCells count="7">
@@ -17893,7 +18318,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:W22"/>
+  <dimension ref="A1:W23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -19702,6 +20127,30 @@
       <c r="V22" s="17" t="inlineStr"/>
       <c r="W22" s="18" t="inlineStr"/>
     </row>
+    <row r="23">
+      <c r="B23" s="19" t="n"/>
+      <c r="C23" s="19" t="n"/>
+      <c r="D23" s="19" t="n"/>
+      <c r="E23" s="19" t="n"/>
+      <c r="F23" s="19" t="n"/>
+      <c r="G23" s="19" t="n"/>
+      <c r="H23" s="19" t="n"/>
+      <c r="I23" s="19" t="n"/>
+      <c r="J23" s="19" t="n"/>
+      <c r="K23" s="19" t="n"/>
+      <c r="L23" s="19" t="n"/>
+      <c r="M23" s="19" t="n"/>
+      <c r="N23" s="19" t="n"/>
+      <c r="O23" s="19" t="n"/>
+      <c r="P23" s="19" t="n"/>
+      <c r="Q23" s="19" t="n"/>
+      <c r="R23" s="19" t="n"/>
+      <c r="S23" s="19" t="n"/>
+      <c r="T23" s="19" t="n"/>
+      <c r="U23" s="19" t="n"/>
+      <c r="V23" s="19" t="n"/>
+      <c r="W23" s="19" t="n"/>
+    </row>
   </sheetData>
   <mergeCells count="15">
     <mergeCell ref="B9:B10"/>
@@ -19730,7 +20179,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:W24"/>
+  <dimension ref="A1:W25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -21537,6 +21986,30 @@
       <c r="V24" s="17" t="inlineStr"/>
       <c r="W24" s="18" t="inlineStr"/>
     </row>
+    <row r="25">
+      <c r="B25" s="19" t="n"/>
+      <c r="C25" s="19" t="n"/>
+      <c r="D25" s="19" t="n"/>
+      <c r="E25" s="19" t="n"/>
+      <c r="F25" s="19" t="n"/>
+      <c r="G25" s="19" t="n"/>
+      <c r="H25" s="19" t="n"/>
+      <c r="I25" s="19" t="n"/>
+      <c r="J25" s="19" t="n"/>
+      <c r="K25" s="19" t="n"/>
+      <c r="L25" s="19" t="n"/>
+      <c r="M25" s="19" t="n"/>
+      <c r="N25" s="19" t="n"/>
+      <c r="O25" s="19" t="n"/>
+      <c r="P25" s="19" t="n"/>
+      <c r="Q25" s="19" t="n"/>
+      <c r="R25" s="19" t="n"/>
+      <c r="S25" s="19" t="n"/>
+      <c r="T25" s="19" t="n"/>
+      <c r="U25" s="19" t="n"/>
+      <c r="V25" s="19" t="n"/>
+      <c r="W25" s="19" t="n"/>
+    </row>
   </sheetData>
   <mergeCells count="15">
     <mergeCell ref="B9:B10"/>
@@ -21565,7 +22038,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:W19"/>
+  <dimension ref="A1:W20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -22948,78 +23421,102 @@
     </row>
     <row r="19" ht="14.3" customHeight="1">
       <c r="A19" s="2" t="n"/>
-      <c r="B19" s="19" t="n">
+      <c r="B19" s="20" t="n">
         <v>9</v>
       </c>
-      <c r="C19" s="19" t="inlineStr">
+      <c r="C19" s="20" t="inlineStr">
         <is>
           <t>15:00-15:45</t>
         </is>
       </c>
-      <c r="D19" s="20" t="inlineStr">
+      <c r="D19" s="21" t="inlineStr">
         <is>
           <t>w.f</t>
         </is>
       </c>
-      <c r="E19" s="20" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="F19" s="20" t="inlineStr">
+      <c r="E19" s="21" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F19" s="21" t="inlineStr">
         <is>
           <t>RB</t>
         </is>
       </c>
-      <c r="G19" s="21" t="inlineStr">
+      <c r="G19" s="22" t="inlineStr">
         <is>
           <t>s1</t>
         </is>
       </c>
-      <c r="H19" s="20" t="inlineStr"/>
-      <c r="I19" s="20" t="inlineStr"/>
-      <c r="J19" s="20" t="inlineStr"/>
-      <c r="K19" s="21" t="inlineStr"/>
-      <c r="L19" s="20" t="inlineStr"/>
-      <c r="M19" s="20" t="inlineStr"/>
-      <c r="N19" s="20" t="inlineStr"/>
-      <c r="O19" s="21" t="inlineStr"/>
-      <c r="P19" s="20" t="inlineStr">
+      <c r="H19" s="21" t="inlineStr"/>
+      <c r="I19" s="21" t="inlineStr"/>
+      <c r="J19" s="21" t="inlineStr"/>
+      <c r="K19" s="22" t="inlineStr"/>
+      <c r="L19" s="21" t="inlineStr"/>
+      <c r="M19" s="21" t="inlineStr"/>
+      <c r="N19" s="21" t="inlineStr"/>
+      <c r="O19" s="22" t="inlineStr"/>
+      <c r="P19" s="21" t="inlineStr">
         <is>
           <t>geografia</t>
         </is>
       </c>
-      <c r="Q19" s="20" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="R19" s="20" t="inlineStr">
+      <c r="Q19" s="21" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="R19" s="21" t="inlineStr">
         <is>
           <t>KR</t>
         </is>
       </c>
-      <c r="S19" s="21" t="n">
+      <c r="S19" s="22" t="n">
         <v>103</v>
       </c>
-      <c r="T19" s="20" t="inlineStr">
+      <c r="T19" s="21" t="inlineStr">
         <is>
           <t>religia</t>
         </is>
       </c>
-      <c r="U19" s="20" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="V19" s="20" t="inlineStr">
+      <c r="U19" s="21" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="V19" s="21" t="inlineStr">
         <is>
           <t>#re2</t>
         </is>
       </c>
-      <c r="W19" s="21" t="n">
+      <c r="W19" s="22" t="n">
         <v>115</v>
       </c>
+    </row>
+    <row r="20">
+      <c r="B20" s="19" t="n"/>
+      <c r="C20" s="19" t="n"/>
+      <c r="D20" s="19" t="n"/>
+      <c r="E20" s="19" t="n"/>
+      <c r="F20" s="19" t="n"/>
+      <c r="G20" s="19" t="n"/>
+      <c r="H20" s="19" t="n"/>
+      <c r="I20" s="19" t="n"/>
+      <c r="J20" s="19" t="n"/>
+      <c r="K20" s="19" t="n"/>
+      <c r="L20" s="19" t="n"/>
+      <c r="M20" s="19" t="n"/>
+      <c r="N20" s="19" t="n"/>
+      <c r="O20" s="19" t="n"/>
+      <c r="P20" s="19" t="n"/>
+      <c r="Q20" s="19" t="n"/>
+      <c r="R20" s="19" t="n"/>
+      <c r="S20" s="19" t="n"/>
+      <c r="T20" s="19" t="n"/>
+      <c r="U20" s="19" t="n"/>
+      <c r="V20" s="19" t="n"/>
+      <c r="W20" s="19" t="n"/>
     </row>
   </sheetData>
   <mergeCells count="13">
@@ -23047,7 +23544,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:W18"/>
+  <dimension ref="A1:W19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -24383,62 +24880,86 @@
     </row>
     <row r="18" ht="14.3" customHeight="1">
       <c r="A18" s="2" t="n"/>
-      <c r="B18" s="19" t="n">
+      <c r="B18" s="20" t="n">
         <v>9</v>
       </c>
-      <c r="C18" s="19" t="inlineStr">
+      <c r="C18" s="20" t="inlineStr">
         <is>
           <t>15:00-15:45</t>
         </is>
       </c>
-      <c r="D18" s="20" t="inlineStr">
+      <c r="D18" s="21" t="inlineStr">
         <is>
           <t>zab.maj</t>
         </is>
       </c>
-      <c r="E18" s="20" t="inlineStr">
+      <c r="E18" s="21" t="inlineStr">
         <is>
           <t>log</t>
         </is>
       </c>
-      <c r="F18" s="20" t="inlineStr">
+      <c r="F18" s="21" t="inlineStr">
         <is>
           <t>MŚ</t>
         </is>
       </c>
-      <c r="G18" s="21" t="n">
+      <c r="G18" s="22" t="n">
         <v>109</v>
       </c>
-      <c r="H18" s="20" t="inlineStr">
+      <c r="H18" s="21" t="inlineStr">
         <is>
           <t>religia</t>
         </is>
       </c>
-      <c r="I18" s="20" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="J18" s="20" t="inlineStr">
+      <c r="I18" s="21" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="J18" s="21" t="inlineStr">
         <is>
           <t>SM</t>
         </is>
       </c>
-      <c r="K18" s="21" t="n">
+      <c r="K18" s="22" t="n">
         <v>116</v>
       </c>
-      <c r="L18" s="20" t="inlineStr"/>
-      <c r="M18" s="20" t="inlineStr"/>
-      <c r="N18" s="20" t="inlineStr"/>
-      <c r="O18" s="21" t="inlineStr"/>
-      <c r="P18" s="20" t="inlineStr"/>
-      <c r="Q18" s="20" t="inlineStr"/>
-      <c r="R18" s="20" t="inlineStr"/>
-      <c r="S18" s="21" t="inlineStr"/>
-      <c r="T18" s="20" t="inlineStr"/>
-      <c r="U18" s="20" t="inlineStr"/>
-      <c r="V18" s="20" t="inlineStr"/>
-      <c r="W18" s="21" t="inlineStr"/>
+      <c r="L18" s="21" t="inlineStr"/>
+      <c r="M18" s="21" t="inlineStr"/>
+      <c r="N18" s="21" t="inlineStr"/>
+      <c r="O18" s="22" t="inlineStr"/>
+      <c r="P18" s="21" t="inlineStr"/>
+      <c r="Q18" s="21" t="inlineStr"/>
+      <c r="R18" s="21" t="inlineStr"/>
+      <c r="S18" s="22" t="inlineStr"/>
+      <c r="T18" s="21" t="inlineStr"/>
+      <c r="U18" s="21" t="inlineStr"/>
+      <c r="V18" s="21" t="inlineStr"/>
+      <c r="W18" s="22" t="inlineStr"/>
+    </row>
+    <row r="19">
+      <c r="B19" s="19" t="n"/>
+      <c r="C19" s="19" t="n"/>
+      <c r="D19" s="19" t="n"/>
+      <c r="E19" s="19" t="n"/>
+      <c r="F19" s="19" t="n"/>
+      <c r="G19" s="19" t="n"/>
+      <c r="H19" s="19" t="n"/>
+      <c r="I19" s="19" t="n"/>
+      <c r="J19" s="19" t="n"/>
+      <c r="K19" s="19" t="n"/>
+      <c r="L19" s="19" t="n"/>
+      <c r="M19" s="19" t="n"/>
+      <c r="N19" s="19" t="n"/>
+      <c r="O19" s="19" t="n"/>
+      <c r="P19" s="19" t="n"/>
+      <c r="Q19" s="19" t="n"/>
+      <c r="R19" s="19" t="n"/>
+      <c r="S19" s="19" t="n"/>
+      <c r="T19" s="19" t="n"/>
+      <c r="U19" s="19" t="n"/>
+      <c r="V19" s="19" t="n"/>
+      <c r="W19" s="19" t="n"/>
     </row>
   </sheetData>
   <mergeCells count="12">
@@ -24465,7 +24986,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:W17"/>
+  <dimension ref="A1:W18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -25356,50 +25877,74 @@
     </row>
     <row r="17" ht="14.3" customHeight="1">
       <c r="A17" s="2" t="n"/>
-      <c r="B17" s="19" t="n">
+      <c r="B17" s="20" t="n">
         <v>9</v>
       </c>
-      <c r="C17" s="19" t="inlineStr">
+      <c r="C17" s="20" t="inlineStr">
         <is>
           <t>15:00-15:45</t>
         </is>
       </c>
-      <c r="D17" s="20" t="inlineStr"/>
-      <c r="E17" s="20" t="inlineStr"/>
-      <c r="F17" s="20" t="inlineStr"/>
-      <c r="G17" s="21" t="inlineStr"/>
-      <c r="H17" s="20" t="inlineStr"/>
-      <c r="I17" s="20" t="inlineStr"/>
-      <c r="J17" s="20" t="inlineStr"/>
-      <c r="K17" s="21" t="inlineStr"/>
-      <c r="L17" s="20" t="inlineStr"/>
-      <c r="M17" s="20" t="inlineStr"/>
-      <c r="N17" s="20" t="inlineStr"/>
-      <c r="O17" s="21" t="inlineStr"/>
-      <c r="P17" s="20" t="inlineStr">
+      <c r="D17" s="21" t="inlineStr"/>
+      <c r="E17" s="21" t="inlineStr"/>
+      <c r="F17" s="21" t="inlineStr"/>
+      <c r="G17" s="22" t="inlineStr"/>
+      <c r="H17" s="21" t="inlineStr"/>
+      <c r="I17" s="21" t="inlineStr"/>
+      <c r="J17" s="21" t="inlineStr"/>
+      <c r="K17" s="22" t="inlineStr"/>
+      <c r="L17" s="21" t="inlineStr"/>
+      <c r="M17" s="21" t="inlineStr"/>
+      <c r="N17" s="21" t="inlineStr"/>
+      <c r="O17" s="22" t="inlineStr"/>
+      <c r="P17" s="21" t="inlineStr">
         <is>
           <t>w.f</t>
         </is>
       </c>
-      <c r="Q17" s="20" t="inlineStr">
+      <c r="Q17" s="21" t="inlineStr">
         <is>
           <t>j1</t>
         </is>
       </c>
-      <c r="R17" s="20" t="inlineStr">
+      <c r="R17" s="21" t="inlineStr">
         <is>
           <t>RB</t>
         </is>
       </c>
-      <c r="S17" s="21" t="inlineStr">
+      <c r="S17" s="22" t="inlineStr">
         <is>
           <t>s1</t>
         </is>
       </c>
-      <c r="T17" s="20" t="inlineStr"/>
-      <c r="U17" s="20" t="inlineStr"/>
-      <c r="V17" s="20" t="inlineStr"/>
-      <c r="W17" s="21" t="inlineStr"/>
+      <c r="T17" s="21" t="inlineStr"/>
+      <c r="U17" s="21" t="inlineStr"/>
+      <c r="V17" s="21" t="inlineStr"/>
+      <c r="W17" s="22" t="inlineStr"/>
+    </row>
+    <row r="18">
+      <c r="B18" s="19" t="n"/>
+      <c r="C18" s="19" t="n"/>
+      <c r="D18" s="19" t="n"/>
+      <c r="E18" s="19" t="n"/>
+      <c r="F18" s="19" t="n"/>
+      <c r="G18" s="19" t="n"/>
+      <c r="H18" s="19" t="n"/>
+      <c r="I18" s="19" t="n"/>
+      <c r="J18" s="19" t="n"/>
+      <c r="K18" s="19" t="n"/>
+      <c r="L18" s="19" t="n"/>
+      <c r="M18" s="19" t="n"/>
+      <c r="N18" s="19" t="n"/>
+      <c r="O18" s="19" t="n"/>
+      <c r="P18" s="19" t="n"/>
+      <c r="Q18" s="19" t="n"/>
+      <c r="R18" s="19" t="n"/>
+      <c r="S18" s="19" t="n"/>
+      <c r="T18" s="19" t="n"/>
+      <c r="U18" s="19" t="n"/>
+      <c r="V18" s="19" t="n"/>
+      <c r="W18" s="19" t="n"/>
     </row>
   </sheetData>
   <mergeCells count="11">
@@ -25425,7 +25970,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:W25"/>
+  <dimension ref="A1:W26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -27148,48 +27693,72 @@
     </row>
     <row r="25" ht="14.3" customHeight="1">
       <c r="A25" s="2" t="n"/>
-      <c r="B25" s="19" t="n"/>
-      <c r="C25" s="19" t="inlineStr">
+      <c r="B25" s="20" t="n"/>
+      <c r="C25" s="20" t="inlineStr">
         <is>
           <t>15:00-15:45</t>
         </is>
       </c>
-      <c r="D25" s="20" t="inlineStr"/>
-      <c r="E25" s="20" t="inlineStr"/>
-      <c r="F25" s="20" t="inlineStr"/>
-      <c r="G25" s="21" t="inlineStr"/>
-      <c r="H25" s="20" t="inlineStr"/>
-      <c r="I25" s="20" t="inlineStr"/>
-      <c r="J25" s="20" t="inlineStr"/>
-      <c r="K25" s="21" t="inlineStr"/>
-      <c r="L25" s="20" t="inlineStr">
+      <c r="D25" s="21" t="inlineStr"/>
+      <c r="E25" s="21" t="inlineStr"/>
+      <c r="F25" s="21" t="inlineStr"/>
+      <c r="G25" s="22" t="inlineStr"/>
+      <c r="H25" s="21" t="inlineStr"/>
+      <c r="I25" s="21" t="inlineStr"/>
+      <c r="J25" s="21" t="inlineStr"/>
+      <c r="K25" s="22" t="inlineStr"/>
+      <c r="L25" s="21" t="inlineStr">
         <is>
           <t>pr.fry</t>
         </is>
       </c>
-      <c r="M25" s="20" t="inlineStr">
+      <c r="M25" s="21" t="inlineStr">
         <is>
           <t>fry</t>
         </is>
       </c>
-      <c r="N25" s="20" t="inlineStr">
+      <c r="N25" s="21" t="inlineStr">
         <is>
           <t>PL</t>
         </is>
       </c>
-      <c r="O25" s="21" t="inlineStr">
+      <c r="O25" s="22" t="inlineStr">
         <is>
           <t>_08</t>
         </is>
       </c>
-      <c r="P25" s="20" t="inlineStr"/>
-      <c r="Q25" s="20" t="inlineStr"/>
-      <c r="R25" s="20" t="inlineStr"/>
-      <c r="S25" s="21" t="inlineStr"/>
-      <c r="T25" s="20" t="inlineStr"/>
-      <c r="U25" s="20" t="inlineStr"/>
-      <c r="V25" s="20" t="inlineStr"/>
-      <c r="W25" s="21" t="inlineStr"/>
+      <c r="P25" s="21" t="inlineStr"/>
+      <c r="Q25" s="21" t="inlineStr"/>
+      <c r="R25" s="21" t="inlineStr"/>
+      <c r="S25" s="22" t="inlineStr"/>
+      <c r="T25" s="21" t="inlineStr"/>
+      <c r="U25" s="21" t="inlineStr"/>
+      <c r="V25" s="21" t="inlineStr"/>
+      <c r="W25" s="22" t="inlineStr"/>
+    </row>
+    <row r="26">
+      <c r="B26" s="19" t="n"/>
+      <c r="C26" s="19" t="n"/>
+      <c r="D26" s="19" t="n"/>
+      <c r="E26" s="19" t="n"/>
+      <c r="F26" s="19" t="n"/>
+      <c r="G26" s="19" t="n"/>
+      <c r="H26" s="19" t="n"/>
+      <c r="I26" s="19" t="n"/>
+      <c r="J26" s="19" t="n"/>
+      <c r="K26" s="19" t="n"/>
+      <c r="L26" s="19" t="n"/>
+      <c r="M26" s="19" t="n"/>
+      <c r="N26" s="19" t="n"/>
+      <c r="O26" s="19" t="n"/>
+      <c r="P26" s="19" t="n"/>
+      <c r="Q26" s="19" t="n"/>
+      <c r="R26" s="19" t="n"/>
+      <c r="S26" s="19" t="n"/>
+      <c r="T26" s="19" t="n"/>
+      <c r="U26" s="19" t="n"/>
+      <c r="V26" s="19" t="n"/>
+      <c r="W26" s="19" t="n"/>
     </row>
   </sheetData>
   <mergeCells count="15">
@@ -27219,7 +27788,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:W26"/>
+  <dimension ref="A1:W27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -29016,6 +29585,30 @@
       <c r="V26" s="17" t="inlineStr"/>
       <c r="W26" s="18" t="inlineStr"/>
     </row>
+    <row r="27">
+      <c r="B27" s="19" t="n"/>
+      <c r="C27" s="19" t="n"/>
+      <c r="D27" s="19" t="n"/>
+      <c r="E27" s="19" t="n"/>
+      <c r="F27" s="19" t="n"/>
+      <c r="G27" s="19" t="n"/>
+      <c r="H27" s="19" t="n"/>
+      <c r="I27" s="19" t="n"/>
+      <c r="J27" s="19" t="n"/>
+      <c r="K27" s="19" t="n"/>
+      <c r="L27" s="19" t="n"/>
+      <c r="M27" s="19" t="n"/>
+      <c r="N27" s="19" t="n"/>
+      <c r="O27" s="19" t="n"/>
+      <c r="P27" s="19" t="n"/>
+      <c r="Q27" s="19" t="n"/>
+      <c r="R27" s="19" t="n"/>
+      <c r="S27" s="19" t="n"/>
+      <c r="T27" s="19" t="n"/>
+      <c r="U27" s="19" t="n"/>
+      <c r="V27" s="19" t="n"/>
+      <c r="W27" s="19" t="n"/>
+    </row>
   </sheetData>
   <mergeCells count="17">
     <mergeCell ref="B23:B24"/>

</xml_diff>